<commit_message>
commit 2: new geniric classes and scripts
</commit_message>
<xml_diff>
--- a/VTiger/TestData/Testdata.xlsx
+++ b/VTiger/TestData/Testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\source\repos\VTiger\VTiger\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF8DB45-CA7A-48D0-A49E-94C103A5BBAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F610EF-5C21-4327-B792-1631560A7464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>CCare</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>http://localhost:8084/</t>
+  </si>
+  <si>
+    <t>homepagelink</t>
+  </si>
+  <si>
+    <t>http://localhost:8084/dashboard/welcome</t>
   </si>
 </sst>
 </file>
@@ -408,15 +414,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19C5B01C-A7DC-4C0E-B319-660B83F47416}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -441,6 +448,14 @@
       </c>
       <c r="B3" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>